<commit_message>
Update main.py to automatically find #of members and #of attendees
</commit_message>
<xml_diff>
--- a/Red Cross Club 2021-22 Hours.xlsx
+++ b/Red Cross Club 2021-22 Hours.xlsx
@@ -57,31 +57,8 @@
     </font>
     <font>
       <name val="Arial"/>
-      <charset val="134"/>
-      <color theme="1"/>
-      <sz val="11"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <name val="Arial"/>
       <charset val="0"/>
-      <color theme="0"/>
-      <sz val="11"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <b val="1"/>
-      <color theme="1"/>
-      <sz val="11"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <b val="1"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FF3F3F76"/>
       <sz val="11"/>
       <scheme val="minor"/>
     </font>
@@ -96,7 +73,29 @@
     <font>
       <name val="Arial"/>
       <charset val="0"/>
+      <color rgb="FF0000FF"/>
+      <sz val="11"/>
+      <u val="single"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <charset val="0"/>
       <color rgb="FFFF0000"/>
+      <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <color theme="0"/>
+      <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <charset val="134"/>
+      <color theme="1"/>
       <sz val="11"/>
       <scheme val="minor"/>
     </font>
@@ -118,31 +117,8 @@
     <font>
       <name val="Arial"/>
       <charset val="0"/>
-      <color rgb="FF006100"/>
-      <sz val="11"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <i val="1"/>
-      <color rgb="FF7F7F7F"/>
-      <sz val="11"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <name val="Arial"/>
-      <charset val="134"/>
       <b val="1"/>
-      <color theme="3"/>
-      <sz val="11"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <b val="1"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FFFFFFFF"/>
       <sz val="11"/>
       <scheme val="minor"/>
     </font>
@@ -151,34 +127,6 @@
       <charset val="0"/>
       <b val="1"/>
       <color rgb="FF3F3F3F"/>
-      <sz val="11"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <color rgb="FF3F3F76"/>
-      <sz val="11"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <color rgb="FF9C0006"/>
-      <sz val="11"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <color rgb="FF9C6500"/>
-      <sz val="11"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <color rgb="FFFA7D00"/>
       <sz val="11"/>
       <scheme val="minor"/>
     </font>
@@ -201,9 +149,61 @@
     <font>
       <name val="Arial"/>
       <charset val="0"/>
-      <color rgb="FF0000FF"/>
+      <b val="1"/>
+      <color theme="1"/>
       <sz val="11"/>
-      <u val="single"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <i val="1"/>
+      <color rgb="FF7F7F7F"/>
+      <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <b val="1"/>
+      <color rgb="FFFA7D00"/>
+      <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <color rgb="FF9C6500"/>
+      <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <charset val="134"/>
+      <b val="1"/>
+      <color theme="3"/>
+      <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <color rgb="FF9C0006"/>
+      <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <color rgb="FFFA7D00"/>
+      <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <color rgb="FF006100"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -228,13 +228,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -246,25 +252,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
+        <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -282,7 +270,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -294,7 +288,115 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -306,109 +408,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -540,12 +540,25 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
+      <top/>
+      <bottom style="medium">
         <color theme="4"/>
       </bottom>
       <diagonal/>
@@ -562,54 +575,6 @@
       </top>
       <bottom style="double">
         <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -631,9 +596,44 @@
     <border>
       <left/>
       <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top/>
       <bottom style="double">
         <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -658,148 +658,148 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="22" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="25" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="31" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="27" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="17" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="20" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="23" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="34" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="33" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="19" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="18" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="16" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="15" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="21" borderId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="13" borderId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="32" borderId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="12" borderId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="33" borderId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="18" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="26" borderId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="15" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="12" borderId="14" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="10" fillId="0" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="32" borderId="18" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="11" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="12" borderId="11" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="26" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="16" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="12" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="10" fillId="0" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="24" borderId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="18" borderId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="23" borderId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="34" borderId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="20" borderId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="19" borderId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="14" borderId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="9" borderId="17" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="5" fillId="0" borderId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="15" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="17" borderId="16" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="9" borderId="16" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="14" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="13" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="5" fillId="0" borderId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="15" borderId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="13" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="12" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="10" fillId="0" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="13" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="14" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="10" fillId="0" borderId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1190,8 +1190,8 @@
   </sheetPr>
   <dimension ref="A1:I204"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A80" workbookViewId="0">
-      <selection activeCell="D96" sqref="D96"/>
+    <sheetView tabSelected="1" topLeftCell="A102" workbookViewId="0">
+      <selection activeCell="A129" sqref="A129:A130"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="14.4285714285714" defaultRowHeight="15.75" customHeight="1"/>
@@ -1222,7 +1222,7 @@
         </is>
       </c>
     </row>
-    <row r="2">
+    <row r="2" ht="12" customHeight="1">
       <c r="A2" s="2" t="inlineStr">
         <is>
           <t>Ameer</t>
@@ -1245,7 +1245,7 @@
       <c r="H2" s="4" t="n"/>
       <c r="I2" s="11" t="n"/>
     </row>
-    <row r="3">
+    <row r="3" ht="12" customHeight="1">
       <c r="A3" s="2" t="inlineStr">
         <is>
           <t>Mohammed</t>
@@ -1257,14 +1257,14 @@
         </is>
       </c>
       <c r="C3" s="2" t="n">
-        <v>0</v>
+        <v>7.5</v>
       </c>
       <c r="F3" s="5" t="n"/>
       <c r="G3" s="6" t="n"/>
       <c r="H3" s="6" t="n"/>
       <c r="I3" s="12" t="n"/>
     </row>
-    <row r="4">
+    <row r="4" ht="12" customHeight="1">
       <c r="A4" s="2" t="inlineStr">
         <is>
           <t xml:space="preserve">John Conor </t>
@@ -1276,10 +1276,10 @@
         </is>
       </c>
       <c r="C4" s="2" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5">
+        <v>8.5</v>
+      </c>
+    </row>
+    <row r="5" ht="12" customHeight="1">
       <c r="A5" s="2" t="inlineStr">
         <is>
           <t>maya</t>
@@ -1291,7 +1291,7 @@
         </is>
       </c>
       <c r="C5" s="2" t="n">
-        <v>1</v>
+        <v>8.5</v>
       </c>
       <c r="F5" s="7" t="inlineStr">
         <is>
@@ -1302,7 +1302,7 @@
       <c r="H5" s="4" t="n"/>
       <c r="I5" s="11" t="n"/>
     </row>
-    <row r="6">
+    <row r="6" ht="12" customHeight="1">
       <c r="A6" s="2" t="inlineStr">
         <is>
           <t>Harini</t>
@@ -1325,7 +1325,7 @@
       <c r="H6" s="6" t="n"/>
       <c r="I6" s="12" t="n"/>
     </row>
-    <row r="7">
+    <row r="7" ht="12" customHeight="1">
       <c r="A7" s="2" t="inlineStr">
         <is>
           <t>Dhoon</t>
@@ -1340,7 +1340,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" ht="12" customHeight="1">
       <c r="A8" s="2" t="inlineStr">
         <is>
           <t>caroline</t>
@@ -1352,10 +1352,10 @@
         </is>
       </c>
       <c r="C8" s="2" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9">
+        <v>8.5</v>
+      </c>
+    </row>
+    <row r="9" ht="12" customHeight="1">
       <c r="A9" s="2" t="inlineStr">
         <is>
           <t>Alexa</t>
@@ -1367,7 +1367,7 @@
         </is>
       </c>
       <c r="C9" s="2" t="n">
-        <v>1</v>
+        <v>8.5</v>
       </c>
       <c r="G9" s="9" t="inlineStr">
         <is>
@@ -1379,7 +1379,7 @@
         <v/>
       </c>
     </row>
-    <row r="10">
+    <row r="10" ht="12" customHeight="1">
       <c r="A10" s="2" t="inlineStr">
         <is>
           <t>Anirudh</t>
@@ -1391,13 +1391,13 @@
         </is>
       </c>
       <c r="C10" s="2" t="n">
-        <v>1</v>
+        <v>8.5</v>
       </c>
       <c r="D10" s="2" t="n">
         <v>2</v>
       </c>
     </row>
-    <row r="11">
+    <row r="11" ht="12" customHeight="1">
       <c r="A11" s="2" t="inlineStr">
         <is>
           <t>Erika</t>
@@ -1409,10 +1409,10 @@
         </is>
       </c>
       <c r="C11" s="2" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12">
+        <v>8.5</v>
+      </c>
+    </row>
+    <row r="12" ht="12" customHeight="1">
       <c r="A12" s="2" t="inlineStr">
         <is>
           <t xml:space="preserve">sonya </t>
@@ -1427,7 +1427,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13">
+    <row r="13" ht="12" customHeight="1">
       <c r="A13" s="2" t="inlineStr">
         <is>
           <t>Farhad</t>
@@ -1439,13 +1439,13 @@
         </is>
       </c>
       <c r="C13" s="2" t="n">
-        <v>1</v>
+        <v>8.5</v>
       </c>
       <c r="D13" s="2" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="14">
+    <row r="14" ht="12" customHeight="1">
       <c r="A14" s="2" t="inlineStr">
         <is>
           <t>Shruti</t>
@@ -1457,10 +1457,10 @@
         </is>
       </c>
       <c r="C14" s="2" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15">
+        <v>8.5</v>
+      </c>
+    </row>
+    <row r="15" ht="12" customHeight="1">
       <c r="A15" s="2" t="inlineStr">
         <is>
           <t>Zaila</t>
@@ -1472,13 +1472,13 @@
         </is>
       </c>
       <c r="C15" s="2" t="n">
-        <v>1</v>
+        <v>8.5</v>
       </c>
       <c r="D15" s="2" t="n">
         <v>2</v>
       </c>
     </row>
-    <row r="16">
+    <row r="16" ht="12" customHeight="1">
       <c r="A16" s="2" t="inlineStr">
         <is>
           <t>Jadon</t>
@@ -1496,7 +1496,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17">
+    <row r="17" ht="12" customHeight="1">
       <c r="A17" s="2" t="inlineStr">
         <is>
           <t>Alex</t>
@@ -1508,10 +1508,10 @@
         </is>
       </c>
       <c r="C17" s="2" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18">
+        <v>8.5</v>
+      </c>
+    </row>
+    <row r="18" ht="12" customHeight="1">
       <c r="A18" s="2" t="inlineStr">
         <is>
           <t>Agatha</t>
@@ -1526,7 +1526,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19">
+    <row r="19" ht="12" customHeight="1">
       <c r="A19" s="2" t="inlineStr">
         <is>
           <t>Bianca</t>
@@ -1541,7 +1541,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20">
+    <row r="20" ht="12" customHeight="1">
       <c r="A20" s="2" t="inlineStr">
         <is>
           <t>Shiwon</t>
@@ -1553,10 +1553,10 @@
         </is>
       </c>
       <c r="C20" s="2" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21">
+        <v>7.5</v>
+      </c>
+    </row>
+    <row r="21" ht="12" customHeight="1">
       <c r="A21" s="2" t="inlineStr">
         <is>
           <t>Braxton</t>
@@ -1571,7 +1571,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22">
+    <row r="22" ht="12" customHeight="1">
       <c r="A22" s="2" t="inlineStr">
         <is>
           <t>Gloria</t>
@@ -1583,13 +1583,13 @@
         </is>
       </c>
       <c r="C22" s="2" t="n">
-        <v>0</v>
+        <v>7.5</v>
       </c>
       <c r="D22" s="2" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="23">
+    <row r="23" ht="12" customHeight="1">
       <c r="A23" s="2" t="inlineStr">
         <is>
           <t>Arpita</t>
@@ -1604,7 +1604,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24">
+    <row r="24" ht="12" customHeight="1">
       <c r="A24" s="2" t="inlineStr">
         <is>
           <t xml:space="preserve">Claire </t>
@@ -1619,7 +1619,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25">
+    <row r="25" ht="12" customHeight="1">
       <c r="A25" s="2" t="inlineStr">
         <is>
           <t xml:space="preserve">gabriella </t>
@@ -1631,10 +1631,10 @@
         </is>
       </c>
       <c r="C25" s="2" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26">
+        <v>7.5</v>
+      </c>
+    </row>
+    <row r="26" ht="12" customHeight="1">
       <c r="A26" s="2" t="inlineStr">
         <is>
           <t>Emma</t>
@@ -1649,7 +1649,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27">
+    <row r="27" ht="12" customHeight="1">
       <c r="A27" s="2" t="inlineStr">
         <is>
           <t>Brielle</t>
@@ -1664,7 +1664,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28">
+    <row r="28" ht="12" customHeight="1">
       <c r="A28" s="2" t="inlineStr">
         <is>
           <t>Alyssa</t>
@@ -1676,10 +1676,10 @@
         </is>
       </c>
       <c r="C28" s="2" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="29">
+        <v>8.5</v>
+      </c>
+    </row>
+    <row r="29" ht="12" customHeight="1">
       <c r="A29" s="2" t="inlineStr">
         <is>
           <t xml:space="preserve">Caroline </t>
@@ -1694,7 +1694,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30">
+    <row r="30" ht="12" customHeight="1">
       <c r="A30" s="2" t="inlineStr">
         <is>
           <t>Reem</t>
@@ -1706,10 +1706,10 @@
         </is>
       </c>
       <c r="C30" s="2" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31">
+        <v>7.5</v>
+      </c>
+    </row>
+    <row r="31" ht="12" customHeight="1">
       <c r="A31" s="2" t="inlineStr">
         <is>
           <t>Aditi</t>
@@ -1721,10 +1721,10 @@
         </is>
       </c>
       <c r="C31" s="2" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="32">
+        <v>8.5</v>
+      </c>
+    </row>
+    <row r="32" ht="12" customHeight="1">
       <c r="A32" s="2" t="inlineStr">
         <is>
           <t>Pallav</t>
@@ -1736,10 +1736,10 @@
         </is>
       </c>
       <c r="C32" s="2" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33">
+        <v>7.5</v>
+      </c>
+    </row>
+    <row r="33" ht="12" customHeight="1">
       <c r="A33" s="2" t="inlineStr">
         <is>
           <t>Gargi</t>
@@ -1751,10 +1751,10 @@
         </is>
       </c>
       <c r="C33" s="2" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="34">
+        <v>8.5</v>
+      </c>
+    </row>
+    <row r="34" ht="12" customHeight="1">
       <c r="A34" s="2" t="inlineStr">
         <is>
           <t>Drithi</t>
@@ -1769,7 +1769,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35">
+    <row r="35" ht="12" customHeight="1">
       <c r="A35" s="2" t="inlineStr">
         <is>
           <t>Sofía</t>
@@ -1784,7 +1784,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36">
+    <row r="36" ht="12" customHeight="1">
       <c r="A36" s="2" t="inlineStr">
         <is>
           <t>Ishaanvi</t>
@@ -1796,10 +1796,10 @@
         </is>
       </c>
       <c r="C36" s="2" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37">
+        <v>7.5</v>
+      </c>
+    </row>
+    <row r="37" ht="12" customHeight="1">
       <c r="A37" s="2" t="inlineStr">
         <is>
           <t>eesha</t>
@@ -1814,7 +1814,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38">
+    <row r="38" ht="12" customHeight="1">
       <c r="A38" s="2" t="inlineStr">
         <is>
           <t>Abhinav</t>
@@ -1826,10 +1826,10 @@
         </is>
       </c>
       <c r="C38" s="2" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="39">
+        <v>7.5</v>
+      </c>
+    </row>
+    <row r="39" ht="12" customHeight="1">
       <c r="A39" s="2" t="inlineStr">
         <is>
           <t>Yeonwoo</t>
@@ -1841,10 +1841,10 @@
         </is>
       </c>
       <c r="C39" s="2" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="40">
+        <v>7.5</v>
+      </c>
+    </row>
+    <row r="40" ht="12" customHeight="1">
       <c r="A40" s="2" t="inlineStr">
         <is>
           <t>Rhea</t>
@@ -1859,7 +1859,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41">
+    <row r="41" ht="12" customHeight="1">
       <c r="A41" s="2" t="inlineStr">
         <is>
           <t>Vikrama Chandra</t>
@@ -1874,7 +1874,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42">
+    <row r="42" ht="12" customHeight="1">
       <c r="A42" s="2" t="inlineStr">
         <is>
           <t>Yaewon</t>
@@ -1886,10 +1886,10 @@
         </is>
       </c>
       <c r="C42" s="2" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="43">
+        <v>8.5</v>
+      </c>
+    </row>
+    <row r="43" ht="12" customHeight="1">
       <c r="A43" s="2" t="inlineStr">
         <is>
           <t>Yogya</t>
@@ -1904,7 +1904,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44">
+    <row r="44" ht="12" customHeight="1">
       <c r="A44" s="2" t="inlineStr">
         <is>
           <t>Emma</t>
@@ -1919,7 +1919,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45">
+    <row r="45" ht="12" customHeight="1">
       <c r="A45" s="2" t="inlineStr">
         <is>
           <t>madelyn</t>
@@ -1931,10 +1931,10 @@
         </is>
       </c>
       <c r="C45" s="2" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="46">
+        <v>8.5</v>
+      </c>
+    </row>
+    <row r="46" ht="12" customHeight="1">
       <c r="A46" s="2" t="inlineStr">
         <is>
           <t>Oviya</t>
@@ -1946,10 +1946,10 @@
         </is>
       </c>
       <c r="C46" s="2" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="47">
+        <v>8.5</v>
+      </c>
+    </row>
+    <row r="47" ht="12" customHeight="1">
       <c r="A47" s="2" t="inlineStr">
         <is>
           <t>Ashley</t>
@@ -1964,7 +1964,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48">
+    <row r="48" ht="12" customHeight="1">
       <c r="A48" s="2" t="inlineStr">
         <is>
           <t>Manyu</t>
@@ -1976,10 +1976,10 @@
         </is>
       </c>
       <c r="C48" s="2" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="49">
+        <v>7.5</v>
+      </c>
+    </row>
+    <row r="49" ht="12" customHeight="1">
       <c r="A49" s="2" t="inlineStr">
         <is>
           <t>Hima</t>
@@ -1991,13 +1991,13 @@
         </is>
       </c>
       <c r="C49" s="2" t="n">
-        <v>1</v>
+        <v>8.5</v>
       </c>
       <c r="D49" s="2" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="50">
+    <row r="50" ht="12" customHeight="1">
       <c r="A50" s="2" t="inlineStr">
         <is>
           <t>Sai Harshini</t>
@@ -2009,10 +2009,10 @@
         </is>
       </c>
       <c r="C50" s="2" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="51">
+        <v>8.5</v>
+      </c>
+    </row>
+    <row r="51" ht="12" customHeight="1">
       <c r="A51" s="2" t="inlineStr">
         <is>
           <t xml:space="preserve">Armaan </t>
@@ -2024,10 +2024,10 @@
         </is>
       </c>
       <c r="C51" s="2" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="52">
+        <v>8.5</v>
+      </c>
+    </row>
+    <row r="52" ht="12" customHeight="1">
       <c r="A52" s="2" t="inlineStr">
         <is>
           <t xml:space="preserve">Mackenzie </t>
@@ -2039,10 +2039,10 @@
         </is>
       </c>
       <c r="C52" s="2" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="53">
+        <v>8.5</v>
+      </c>
+    </row>
+    <row r="53" ht="12" customHeight="1">
       <c r="A53" s="2" t="inlineStr">
         <is>
           <t xml:space="preserve">Eba </t>
@@ -2054,10 +2054,10 @@
         </is>
       </c>
       <c r="C53" s="2" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="54">
+        <v>8.5</v>
+      </c>
+    </row>
+    <row r="54" ht="12" customHeight="1">
       <c r="A54" s="2" t="inlineStr">
         <is>
           <t xml:space="preserve">Akhil </t>
@@ -2069,10 +2069,10 @@
         </is>
       </c>
       <c r="C54" s="2" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="55">
+        <v>7.5</v>
+      </c>
+    </row>
+    <row r="55" ht="12" customHeight="1">
       <c r="A55" s="2" t="inlineStr">
         <is>
           <t>Maria</t>
@@ -2087,7 +2087,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56">
+    <row r="56" ht="12" customHeight="1">
       <c r="A56" s="2" t="inlineStr">
         <is>
           <t xml:space="preserve">Daniel </t>
@@ -2099,10 +2099,10 @@
         </is>
       </c>
       <c r="C56" s="2" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="57">
+        <v>8.5</v>
+      </c>
+    </row>
+    <row r="57" ht="12" customHeight="1">
       <c r="A57" s="2" t="inlineStr">
         <is>
           <t>Serena</t>
@@ -2117,7 +2117,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58">
+    <row r="58" ht="12" customHeight="1">
       <c r="A58" s="2" t="inlineStr">
         <is>
           <t>Aanathi</t>
@@ -2132,7 +2132,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="59">
+    <row r="59" ht="12" customHeight="1">
       <c r="A59" s="2" t="inlineStr">
         <is>
           <t>Srijan</t>
@@ -2144,10 +2144,10 @@
         </is>
       </c>
       <c r="C59" s="2" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="60">
+        <v>8.5</v>
+      </c>
+    </row>
+    <row r="60" ht="12" customHeight="1">
       <c r="A60" s="2" t="inlineStr">
         <is>
           <t>Gabby</t>
@@ -2162,7 +2162,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="61">
+    <row r="61" ht="12" customHeight="1">
       <c r="A61" s="2" t="inlineStr">
         <is>
           <t>Sneha</t>
@@ -2177,7 +2177,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="62">
+    <row r="62" ht="12" customHeight="1">
       <c r="A62" s="2" t="inlineStr">
         <is>
           <t>Pavithran</t>
@@ -2189,10 +2189,10 @@
         </is>
       </c>
       <c r="C62" s="2" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="63">
+        <v>8.5</v>
+      </c>
+    </row>
+    <row r="63" ht="12" customHeight="1">
       <c r="A63" s="2" t="inlineStr">
         <is>
           <t>Rhia</t>
@@ -2207,7 +2207,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64">
+    <row r="64" ht="12" customHeight="1">
       <c r="A64" s="2" t="inlineStr">
         <is>
           <t xml:space="preserve">Krish </t>
@@ -2219,10 +2219,10 @@
         </is>
       </c>
       <c r="C64" s="2" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="65">
+        <v>8.5</v>
+      </c>
+    </row>
+    <row r="65" ht="12" customHeight="1">
       <c r="A65" s="2" t="inlineStr">
         <is>
           <t>Om</t>
@@ -2234,10 +2234,10 @@
         </is>
       </c>
       <c r="C65" s="2" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="66">
+        <v>8.5</v>
+      </c>
+    </row>
+    <row r="66" ht="12" customHeight="1">
       <c r="A66" s="2" t="inlineStr">
         <is>
           <t>Sonia</t>
@@ -2249,10 +2249,10 @@
         </is>
       </c>
       <c r="C66" s="2" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="67">
+        <v>8.5</v>
+      </c>
+    </row>
+    <row r="67" ht="12" customHeight="1">
       <c r="A67" s="2" t="inlineStr">
         <is>
           <t>Aadi</t>
@@ -2264,10 +2264,10 @@
         </is>
       </c>
       <c r="C67" s="2" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="68">
+        <v>7.5</v>
+      </c>
+    </row>
+    <row r="68" ht="12" customHeight="1">
       <c r="A68" s="2" t="inlineStr">
         <is>
           <t>Chase</t>
@@ -2279,10 +2279,10 @@
         </is>
       </c>
       <c r="C68" s="2" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="69">
+        <v>7.5</v>
+      </c>
+    </row>
+    <row r="69" ht="12" customHeight="1">
       <c r="A69" s="2" t="inlineStr">
         <is>
           <t>pelmo</t>
@@ -2294,10 +2294,10 @@
         </is>
       </c>
       <c r="C69" s="2" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="70">
+        <v>8.5</v>
+      </c>
+    </row>
+    <row r="70" ht="12" customHeight="1">
       <c r="A70" s="2" t="inlineStr">
         <is>
           <t>Priya</t>
@@ -2309,10 +2309,10 @@
         </is>
       </c>
       <c r="C70" s="2" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="71">
+        <v>8.5</v>
+      </c>
+    </row>
+    <row r="71" ht="12" customHeight="1">
       <c r="A71" s="2" t="inlineStr">
         <is>
           <t xml:space="preserve">Koolsoom </t>
@@ -2324,10 +2324,10 @@
         </is>
       </c>
       <c r="C71" s="2" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="72">
+        <v>7.5</v>
+      </c>
+    </row>
+    <row r="72" ht="12" customHeight="1">
       <c r="A72" s="2" t="inlineStr">
         <is>
           <t>Nasi</t>
@@ -2339,10 +2339,10 @@
         </is>
       </c>
       <c r="C72" s="2" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="73">
+        <v>7.5</v>
+      </c>
+    </row>
+    <row r="73" ht="12" customHeight="1">
       <c r="A73" s="2" t="inlineStr">
         <is>
           <t>Nabiha</t>
@@ -2357,7 +2357,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="74">
+    <row r="74" ht="12" customHeight="1">
       <c r="A74" s="2" t="inlineStr">
         <is>
           <t xml:space="preserve">Amogh </t>
@@ -2369,10 +2369,10 @@
         </is>
       </c>
       <c r="C74" s="2" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="75">
+        <v>8.5</v>
+      </c>
+    </row>
+    <row r="75" ht="12" customHeight="1">
       <c r="A75" s="2" t="inlineStr">
         <is>
           <t>Shravan</t>
@@ -2387,7 +2387,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76">
+    <row r="76" ht="12" customHeight="1">
       <c r="A76" s="2" t="inlineStr">
         <is>
           <t xml:space="preserve">Xingjian </t>
@@ -2402,7 +2402,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77">
+    <row r="77" ht="12" customHeight="1">
       <c r="A77" s="2" t="inlineStr">
         <is>
           <t>Henry</t>
@@ -2417,7 +2417,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78">
+    <row r="78" ht="12" customHeight="1">
       <c r="A78" s="2" t="inlineStr">
         <is>
           <t>Hitha</t>
@@ -2429,10 +2429,10 @@
         </is>
       </c>
       <c r="C78" s="2" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="79">
+        <v>8.5</v>
+      </c>
+    </row>
+    <row r="79" ht="12" customHeight="1">
       <c r="A79" s="2" t="inlineStr">
         <is>
           <t>Ashmeet</t>
@@ -2444,13 +2444,13 @@
         </is>
       </c>
       <c r="C79" s="2" t="n">
-        <v>1</v>
+        <v>8.5</v>
       </c>
       <c r="D79" s="2" t="n">
         <v>2</v>
       </c>
     </row>
-    <row r="80">
+    <row r="80" ht="12" customHeight="1">
       <c r="A80" s="2" t="inlineStr">
         <is>
           <t>Jai</t>
@@ -2465,7 +2465,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="81">
+    <row r="81" ht="12" customHeight="1">
       <c r="A81" s="2" t="inlineStr">
         <is>
           <t xml:space="preserve">Gabriella </t>
@@ -2477,10 +2477,10 @@
         </is>
       </c>
       <c r="C81" s="2" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="82">
+        <v>7.5</v>
+      </c>
+    </row>
+    <row r="82" ht="12" customHeight="1">
       <c r="A82" s="2" t="inlineStr">
         <is>
           <t>kate</t>
@@ -2492,10 +2492,10 @@
         </is>
       </c>
       <c r="C82" s="2" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="83">
+        <v>8.5</v>
+      </c>
+    </row>
+    <row r="83" ht="12" customHeight="1">
       <c r="A83" s="2" t="inlineStr">
         <is>
           <t>Pranathi</t>
@@ -2510,7 +2510,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84">
+    <row r="84" ht="12" customHeight="1">
       <c r="A84" s="2" t="inlineStr">
         <is>
           <t>Neal</t>
@@ -2525,7 +2525,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="85">
+    <row r="85" ht="12" customHeight="1">
       <c r="A85" s="2" t="inlineStr">
         <is>
           <t>Syed</t>
@@ -2540,7 +2540,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="86">
+    <row r="86" ht="12" customHeight="1">
       <c r="A86" s="2" t="inlineStr">
         <is>
           <t>Shaheerah</t>
@@ -2555,7 +2555,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="87">
+    <row r="87" ht="12" customHeight="1">
       <c r="A87" s="2" t="inlineStr">
         <is>
           <t xml:space="preserve">Soumya </t>
@@ -2567,10 +2567,10 @@
         </is>
       </c>
       <c r="C87" s="2" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="88">
+        <v>8.5</v>
+      </c>
+    </row>
+    <row r="88" ht="12" customHeight="1">
       <c r="A88" s="2" t="inlineStr">
         <is>
           <t>Emma</t>
@@ -2582,10 +2582,10 @@
         </is>
       </c>
       <c r="C88" s="2" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="89">
+        <v>8.5</v>
+      </c>
+    </row>
+    <row r="89" ht="12" customHeight="1">
       <c r="A89" s="2" t="inlineStr">
         <is>
           <t>katie</t>
@@ -2597,10 +2597,10 @@
         </is>
       </c>
       <c r="C89" s="2" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="90">
+        <v>7.5</v>
+      </c>
+    </row>
+    <row r="90" ht="12" customHeight="1">
       <c r="A90" s="2" t="inlineStr">
         <is>
           <t>Roshan</t>
@@ -2615,7 +2615,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="91">
+    <row r="91" ht="12" customHeight="1">
       <c r="A91" s="2" t="inlineStr">
         <is>
           <t>Jazmin</t>
@@ -2633,7 +2633,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="92">
+    <row r="92" ht="12" customHeight="1">
       <c r="A92" s="2" t="inlineStr">
         <is>
           <t>Anam</t>
@@ -2645,10 +2645,10 @@
         </is>
       </c>
       <c r="C92" s="2" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="93">
+        <v>8.5</v>
+      </c>
+    </row>
+    <row r="93" ht="12" customHeight="1">
       <c r="A93" s="2" t="inlineStr">
         <is>
           <t xml:space="preserve">Maria </t>
@@ -2660,10 +2660,10 @@
         </is>
       </c>
       <c r="C93" s="2" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="94">
+        <v>8.5</v>
+      </c>
+    </row>
+    <row r="94" ht="12" customHeight="1">
       <c r="A94" s="2" t="inlineStr">
         <is>
           <t>Joven</t>
@@ -2675,10 +2675,10 @@
         </is>
       </c>
       <c r="C94" s="2" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="95">
+        <v>8.5</v>
+      </c>
+    </row>
+    <row r="95" ht="12" customHeight="1">
       <c r="A95" s="2" t="inlineStr">
         <is>
           <t>Emma Kate</t>
@@ -2690,10 +2690,10 @@
         </is>
       </c>
       <c r="C95" s="2" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="96">
+        <v>8.5</v>
+      </c>
+    </row>
+    <row r="96" ht="12" customHeight="1">
       <c r="A96" s="2" t="inlineStr">
         <is>
           <t>Ethan</t>
@@ -2705,10 +2705,10 @@
         </is>
       </c>
       <c r="C96" s="2" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="97">
+        <v>8.5</v>
+      </c>
+    </row>
+    <row r="97" ht="12" customHeight="1">
       <c r="A97" s="2" t="inlineStr">
         <is>
           <t>Ishaan</t>
@@ -2723,7 +2723,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="98">
+    <row r="98" ht="12" customHeight="1">
       <c r="A98" s="2" t="inlineStr">
         <is>
           <t>Yiming</t>
@@ -2738,7 +2738,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="99">
+    <row r="99" ht="12" customHeight="1">
       <c r="A99" s="2" t="inlineStr">
         <is>
           <t>Sufi</t>
@@ -2750,10 +2750,10 @@
         </is>
       </c>
       <c r="C99" s="2" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="100">
+        <v>8.5</v>
+      </c>
+    </row>
+    <row r="100" ht="12" customHeight="1">
       <c r="A100" s="2" t="inlineStr">
         <is>
           <t>Ria</t>
@@ -2768,7 +2768,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="101">
+    <row r="101" ht="12" customHeight="1">
       <c r="A101" s="2" t="inlineStr">
         <is>
           <t>Rithu</t>
@@ -2780,10 +2780,10 @@
         </is>
       </c>
       <c r="C101" s="2" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="102">
+        <v>8.5</v>
+      </c>
+    </row>
+    <row r="102" ht="12" customHeight="1">
       <c r="A102" s="2" t="inlineStr">
         <is>
           <t>Sihi</t>
@@ -2798,7 +2798,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="103">
+    <row r="103" ht="12" customHeight="1">
       <c r="A103" s="2" t="inlineStr">
         <is>
           <t>Anika</t>
@@ -2816,7 +2816,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="104">
+    <row r="104" ht="12" customHeight="1">
       <c r="A104" s="2" t="inlineStr">
         <is>
           <t>Samarth</t>
@@ -2828,13 +2828,13 @@
         </is>
       </c>
       <c r="C104" s="2" t="n">
-        <v>0</v>
+        <v>7.5</v>
       </c>
       <c r="D104" s="2" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="105">
+    <row r="105" ht="12" customHeight="1">
       <c r="A105" s="2" t="inlineStr">
         <is>
           <t>Arnav</t>
@@ -2846,13 +2846,13 @@
         </is>
       </c>
       <c r="C105" s="2" t="n">
-        <v>0</v>
+        <v>7.5</v>
       </c>
       <c r="D105" s="2" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="106">
+    <row r="106" ht="12" customHeight="1">
       <c r="A106" s="2" t="inlineStr">
         <is>
           <t>Katelyn</t>
@@ -2864,10 +2864,10 @@
         </is>
       </c>
       <c r="C106" s="2" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="107">
+        <v>8.5</v>
+      </c>
+    </row>
+    <row r="107" ht="12" customHeight="1">
       <c r="A107" s="2" t="inlineStr">
         <is>
           <t>Addison</t>
@@ -2882,7 +2882,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="108">
+    <row r="108" ht="12" customHeight="1">
       <c r="A108" s="2" t="inlineStr">
         <is>
           <t>Shuoming</t>
@@ -2894,10 +2894,10 @@
         </is>
       </c>
       <c r="C108" s="2" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="109">
+        <v>8.5</v>
+      </c>
+    </row>
+    <row r="109" ht="12" customHeight="1">
       <c r="A109" s="2" t="inlineStr">
         <is>
           <t>Derek</t>
@@ -2909,10 +2909,10 @@
         </is>
       </c>
       <c r="C109" s="2" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="110">
+        <v>8.5</v>
+      </c>
+    </row>
+    <row r="110" ht="12" customHeight="1">
       <c r="A110" s="2" t="inlineStr">
         <is>
           <t>Chavi</t>
@@ -2924,10 +2924,10 @@
         </is>
       </c>
       <c r="C110" s="2" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="111">
+        <v>8.5</v>
+      </c>
+    </row>
+    <row r="111" ht="12" customHeight="1">
       <c r="A111" s="2" t="inlineStr">
         <is>
           <t xml:space="preserve">Trinity </t>
@@ -2939,10 +2939,10 @@
         </is>
       </c>
       <c r="C111" s="2" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="112">
+        <v>8.5</v>
+      </c>
+    </row>
+    <row r="112" ht="12" customHeight="1">
       <c r="A112" s="2" t="inlineStr">
         <is>
           <t>london</t>
@@ -2954,10 +2954,10 @@
         </is>
       </c>
       <c r="C112" s="2" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="113">
+        <v>8.5</v>
+      </c>
+    </row>
+    <row r="113" ht="12" customHeight="1">
       <c r="A113" s="2" t="inlineStr">
         <is>
           <t>Carolyn</t>
@@ -2969,10 +2969,10 @@
         </is>
       </c>
       <c r="C113" s="2" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="114">
+        <v>8.5</v>
+      </c>
+    </row>
+    <row r="114" ht="12" customHeight="1">
       <c r="A114" s="2" t="inlineStr">
         <is>
           <t>Keerti</t>
@@ -2984,10 +2984,10 @@
         </is>
       </c>
       <c r="C114" s="2" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="115">
+        <v>7.5</v>
+      </c>
+    </row>
+    <row r="115" ht="12" customHeight="1">
       <c r="A115" s="2" t="inlineStr">
         <is>
           <t xml:space="preserve">Benjamin </t>
@@ -3002,7 +3002,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="116">
+    <row r="116" ht="12" customHeight="1">
       <c r="A116" s="2" t="inlineStr">
         <is>
           <t>Zhijia</t>
@@ -3017,7 +3017,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="117">
+    <row r="117" ht="12" customHeight="1">
       <c r="A117" s="2" t="inlineStr">
         <is>
           <t>Yujia</t>
@@ -3035,7 +3035,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="118">
+    <row r="118" ht="12" customHeight="1">
       <c r="A118" s="2" t="inlineStr">
         <is>
           <t>Huini</t>
@@ -3053,7 +3053,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="119">
+    <row r="119" ht="12" customHeight="1">
       <c r="A119" s="2" t="inlineStr">
         <is>
           <t>nancee</t>
@@ -3065,10 +3065,10 @@
         </is>
       </c>
       <c r="C119" s="2" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="120">
+        <v>8.5</v>
+      </c>
+    </row>
+    <row r="120" ht="12" customHeight="1">
       <c r="A120" s="2" t="inlineStr">
         <is>
           <t>Joselyn</t>
@@ -3080,10 +3080,10 @@
         </is>
       </c>
       <c r="C120" s="2" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="121">
+        <v>8.5</v>
+      </c>
+    </row>
+    <row r="121" ht="12" customHeight="1">
       <c r="A121" s="2" t="inlineStr">
         <is>
           <t xml:space="preserve">John </t>
@@ -3095,10 +3095,10 @@
         </is>
       </c>
       <c r="C121" s="2" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="122">
+        <v>8.5</v>
+      </c>
+    </row>
+    <row r="122" ht="12" customHeight="1">
       <c r="A122" s="2" t="inlineStr">
         <is>
           <t>Lily</t>
@@ -3113,7 +3113,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="123">
+    <row r="123" ht="12" customHeight="1">
       <c r="A123" s="2" t="inlineStr">
         <is>
           <t>Nicolas</t>

</xml_diff>